<commit_message>
working with user data
</commit_message>
<xml_diff>
--- a/pidsg25-05.xlsx
+++ b/pidsg25-05.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="20">
   <si>
     <t xml:space="preserve">FY24</t>
   </si>
@@ -67,7 +67,22 @@
     <t xml:space="preserve">Material</t>
   </si>
   <si>
+    <t xml:space="preserve">Hedge raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unhedge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gm to toz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedged proc</t>
   </si>
 </sst>
 </file>
@@ -204,7 +219,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,7 +415,7 @@
   <dimension ref="B3:P27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="E5:E16 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="H11:H16 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1368,7 +1383,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="1" sqref="E5:E16 J15"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="1" sqref="H11:H16 J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1818,7 +1833,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="E5:E16 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="H11:H16 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2267,21 +2282,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:E16"/>
+  <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5:E16"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="9" t="n">
         <v>45772</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -2290,13 +2323,24 @@
       <c r="D5" s="1" t="n">
         <v>152000</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <f aca="false">SUM(C5:D5)</f>
         <v>304000</v>
       </c>
+      <c r="F5" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G5" s="10" t="n">
+        <f aca="false">E5/F5</f>
+        <v>9773.66255144033</v>
+      </c>
+      <c r="H5" s="10" t="n">
+        <f aca="false">C5/F5</f>
+        <v>4886.83127572017</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="9" t="n">
         <v>45802</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -2305,13 +2349,24 @@
       <c r="D6" s="1" t="n">
         <v>6000</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <f aca="false">SUM(C6:D6)</f>
         <v>158000</v>
       </c>
+      <c r="F6" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G6" s="10" t="n">
+        <f aca="false">E6/F6</f>
+        <v>5079.73251028807</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <f aca="false">C6/F6</f>
+        <v>4886.83127572017</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="9" t="n">
         <v>45833</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -2320,13 +2375,24 @@
       <c r="D7" s="1" t="n">
         <v>156000</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <f aca="false">SUM(C7:D7)</f>
         <v>308000</v>
       </c>
+      <c r="F7" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <f aca="false">E7/F7</f>
+        <v>9902.2633744856</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <f aca="false">C7/F7</f>
+        <v>4886.83127572017</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="9" t="n">
         <v>45863</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -2335,13 +2401,24 @@
       <c r="D8" s="1" t="n">
         <v>107000</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <f aca="false">SUM(C8:D8)</f>
         <v>259000</v>
       </c>
+      <c r="F8" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <f aca="false">E8/F8</f>
+        <v>8326.90329218107</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <f aca="false">C8/F8</f>
+        <v>4886.83127572017</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="9" t="n">
         <v>45894</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -2350,13 +2427,24 @@
       <c r="D9" s="1" t="n">
         <v>107000</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <f aca="false">SUM(C9:D9)</f>
         <v>259000</v>
       </c>
+      <c r="F9" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <f aca="false">E9/F9</f>
+        <v>8326.90329218107</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <f aca="false">C9/F9</f>
+        <v>4886.83127572017</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="10" t="n">
+      <c r="B10" s="9" t="n">
         <v>45925</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -2365,13 +2453,24 @@
       <c r="D10" s="1" t="n">
         <v>42000</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <f aca="false">SUM(C10:D10)</f>
         <v>194000</v>
       </c>
+      <c r="F10" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <f aca="false">E10/F10</f>
+        <v>6237.13991769547</v>
+      </c>
+      <c r="H10" s="10" t="n">
+        <f aca="false">C10/F10</f>
+        <v>4886.83127572017</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="n">
+      <c r="B11" s="9" t="n">
         <v>45955</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -2380,13 +2479,24 @@
       <c r="D11" s="1" t="n">
         <v>76000</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <f aca="false">SUM(C11:D11)</f>
         <v>162000</v>
       </c>
+      <c r="F11" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <f aca="false">E11/F11</f>
+        <v>5208.33333333333</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <f aca="false">C11/F11</f>
+        <v>2764.91769547325</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="n">
+      <c r="B12" s="9" t="n">
         <v>45986</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -2395,13 +2505,24 @@
       <c r="D12" s="1" t="n">
         <v>107924</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <f aca="false">SUM(C12:D12)</f>
         <v>194000</v>
       </c>
+      <c r="F12" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <f aca="false">E12/F12</f>
+        <v>6237.13991769547</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <f aca="false">C12/F12</f>
+        <v>2767.36111111111</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
+      <c r="B13" s="9" t="n">
         <v>46016</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -2410,13 +2531,24 @@
       <c r="D13" s="1" t="n">
         <v>140924</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <f aca="false">SUM(C13:D13)</f>
         <v>227000</v>
       </c>
+      <c r="F13" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <f aca="false">E13/F13</f>
+        <v>7298.09670781893</v>
+      </c>
+      <c r="H13" s="10" t="n">
+        <f aca="false">C13/F13</f>
+        <v>2767.36111111111</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="n">
+      <c r="B14" s="9" t="n">
         <v>46047</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -2425,13 +2557,24 @@
       <c r="D14" s="1" t="n">
         <v>26924</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <f aca="false">SUM(C14:D14)</f>
         <v>113000</v>
       </c>
+      <c r="F14" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G14" s="10" t="n">
+        <f aca="false">E14/F14</f>
+        <v>3632.97325102881</v>
+      </c>
+      <c r="H14" s="10" t="n">
+        <f aca="false">C14/F14</f>
+        <v>2767.36111111111</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="n">
+      <c r="B15" s="9" t="n">
         <v>46078</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -2440,13 +2583,24 @@
       <c r="D15" s="1" t="n">
         <v>91924</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <f aca="false">SUM(C15:D15)</f>
         <v>178000</v>
       </c>
+      <c r="F15" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G15" s="10" t="n">
+        <f aca="false">E15/F15</f>
+        <v>5722.7366255144</v>
+      </c>
+      <c r="H15" s="10" t="n">
+        <f aca="false">C15/F15</f>
+        <v>2767.36111111111</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="n">
+      <c r="B16" s="9" t="n">
         <v>46106</v>
       </c>
       <c r="C16" s="1" t="n">
@@ -2455,9 +2609,20 @@
       <c r="D16" s="1" t="n">
         <v>75924</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <f aca="false">SUM(C16:D16)</f>
         <v>162000</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>31.104</v>
+      </c>
+      <c r="G16" s="10" t="n">
+        <f aca="false">E16/F16</f>
+        <v>5208.33333333333</v>
+      </c>
+      <c r="H16" s="10" t="n">
+        <f aca="false">C16/F16</f>
+        <v>2767.36111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>